<commit_message>
Moved 32bp spread to the correct side.
(cherry picked from commit 4fa5fbac7a0b3041338227e2233abf3bc288a2a7)
</commit_message>
<xml_diff>
--- a/cl/hackathon/HackathonOutput.xlsx
+++ b/cl/hackathon/HackathonOutput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\AI\Code\TradeEntry\tradeentry-monorepo-2\cl\hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B2DC5F-E93B-4C85-BA48-905529F06CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B40870-C9FE-4F38-B626-73941CC060CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{17967F1D-B68D-43EA-A7AC-51D6C7F5928A}"/>
   </bookViews>
@@ -1035,7 +1035,7 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1480,14 +1480,14 @@
       <c r="J12" t="s">
         <v>32</v>
       </c>
-      <c r="N12">
-        <v>32</v>
-      </c>
       <c r="P12">
         <v>5000000000</v>
       </c>
       <c r="Q12" t="s">
         <v>42</v>
+      </c>
+      <c r="U12">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">

</xml_diff>